<commit_message>
Fixed error where CO2 sequestered was off by 1000x
</commit_message>
<xml_diff>
--- a/InputData/land/CSpULApYbP/CO2 Sequestered per Unit Land Area per Year by Pol.xlsx
+++ b/InputData/land/CSpULApYbP/CO2 Sequestered per Unit Land Area per Year by Pol.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\Brazil\Models\eps-brazil\InputData\land\CSpULApYbP\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="315" yWindow="315" windowWidth="18825" windowHeight="6555"/>
+    <workbookView xWindow="315" yWindow="315" windowWidth="18825" windowHeight="6555" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -22,7 +27,7 @@
     <definedName name="C_to_CO2">'[1]Conversion Factors'!$A$4</definedName>
     <definedName name="grams_per_ton">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -227,7 +232,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -400,7 +405,7 @@
     <cellStyle name="Font: Calibri, 9pt regular" xfId="2"/>
     <cellStyle name="Footnotes: top row" xfId="3"/>
     <cellStyle name="Header: bottom row" xfId="4"/>
-    <cellStyle name="Hiperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Parent row" xfId="5"/>
     <cellStyle name="Table title" xfId="6"/>
@@ -476,9 +481,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -516,9 +521,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -553,7 +558,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -588,7 +593,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -764,7 +769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
@@ -1077,7 +1082,7 @@
   <dimension ref="A2:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1145,7 +1150,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1356,8 +1361,8 @@
   </sheetPr>
   <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B3:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1401,8 +1406,8 @@
         <v>3</v>
       </c>
       <c r="B3" s="3">
-        <f>'Aff &amp; Ref'!B19*1000000</f>
-        <v>2568.140587508688</v>
+        <f>'Aff &amp; Ref'!B19*10^9</f>
+        <v>2568140.5875086877</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1452,8 +1457,8 @@
         <v>5</v>
       </c>
       <c r="B5" s="3">
-        <f>'Avoided Def'!B13*1000000</f>
-        <v>75884.477421999734</v>
+        <f>'Avoided Def'!B13*10^9</f>
+        <v>75884477.421999738</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1537,8 +1542,8 @@
         <v>7</v>
       </c>
       <c r="B7" s="3">
-        <f>'Forest Rest'!B12*1000000</f>
-        <v>1144.0518394431674</v>
+        <f>'Forest Rest'!B12*10^9</f>
+        <v>1144051.8394431674</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>

</xml_diff>

<commit_message>
Revert "Fixed error where CO2 sequestered was off by 1000x"
This reverts commit 2d3d6d28326c05dcbbcb2dbf62859e29fd365583.
</commit_message>
<xml_diff>
--- a/InputData/land/CSpULApYbP/CO2 Sequestered per Unit Land Area per Year by Pol.xlsx
+++ b/InputData/land/CSpULApYbP/CO2 Sequestered per Unit Land Area per Year by Pol.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\Brazil\Models\eps-brazil\InputData\land\CSpULApYbP\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="315" yWindow="315" windowWidth="18825" windowHeight="6555" activeTab="4"/>
+    <workbookView xWindow="315" yWindow="315" windowWidth="18825" windowHeight="6555"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -27,7 +22,7 @@
     <definedName name="C_to_CO2">'[1]Conversion Factors'!$A$4</definedName>
     <definedName name="grams_per_ton">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -232,7 +227,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -405,7 +400,7 @@
     <cellStyle name="Font: Calibri, 9pt regular" xfId="2"/>
     <cellStyle name="Footnotes: top row" xfId="3"/>
     <cellStyle name="Header: bottom row" xfId="4"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="Hiperlink" xfId="7" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Parent row" xfId="5"/>
     <cellStyle name="Table title" xfId="6"/>
@@ -481,9 +476,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -521,9 +516,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -558,7 +553,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -593,7 +588,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -769,7 +764,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
@@ -1082,7 +1077,7 @@
   <dimension ref="A2:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1150,7 +1145,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1361,8 +1356,8 @@
   </sheetPr>
   <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B3:B6"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1406,8 +1401,8 @@
         <v>3</v>
       </c>
       <c r="B3" s="3">
-        <f>'Aff &amp; Ref'!B19*10^9</f>
-        <v>2568140.5875086877</v>
+        <f>'Aff &amp; Ref'!B19*1000000</f>
+        <v>2568.140587508688</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1457,8 +1452,8 @@
         <v>5</v>
       </c>
       <c r="B5" s="3">
-        <f>'Avoided Def'!B13*10^9</f>
-        <v>75884477.421999738</v>
+        <f>'Avoided Def'!B13*1000000</f>
+        <v>75884.477421999734</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1542,8 +1537,8 @@
         <v>7</v>
       </c>
       <c r="B7" s="3">
-        <f>'Forest Rest'!B12*10^9</f>
-        <v>1144051.8394431674</v>
+        <f>'Forest Rest'!B12*1000000</f>
+        <v>1144.0518394431674</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>

</xml_diff>

<commit_message>
Fixes error with sequestration amounts being low by 1000x
</commit_message>
<xml_diff>
--- a/InputData/land/CSpULApYbP/CO2 Sequestered per Unit Land Area per Year by Pol.xlsx
+++ b/InputData/land/CSpULApYbP/CO2 Sequestered per Unit Land Area per Year by Pol.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\Brazil\Models\eps-brazil\InputData\land\CSpULApYbP\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="315" yWindow="315" windowWidth="18825" windowHeight="6555"/>
+    <workbookView xWindow="315" yWindow="315" windowWidth="18825" windowHeight="6555" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -22,7 +27,7 @@
     <definedName name="C_to_CO2">'[1]Conversion Factors'!$A$4</definedName>
     <definedName name="grams_per_ton">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -227,7 +232,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -400,7 +405,7 @@
     <cellStyle name="Font: Calibri, 9pt regular" xfId="2"/>
     <cellStyle name="Footnotes: top row" xfId="3"/>
     <cellStyle name="Header: bottom row" xfId="4"/>
-    <cellStyle name="Hiperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Parent row" xfId="5"/>
     <cellStyle name="Table title" xfId="6"/>
@@ -476,9 +481,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -516,9 +521,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -553,7 +558,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -588,7 +593,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -764,7 +769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
@@ -1077,7 +1082,7 @@
   <dimension ref="A2:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1145,7 +1150,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1356,8 +1361,8 @@
   </sheetPr>
   <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B3:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1401,8 +1406,8 @@
         <v>3</v>
       </c>
       <c r="B3" s="3">
-        <f>'Aff &amp; Ref'!B19*1000000</f>
-        <v>2568.140587508688</v>
+        <f>'Aff &amp; Ref'!B19*10^9</f>
+        <v>2568140.5875086877</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1452,8 +1457,8 @@
         <v>5</v>
       </c>
       <c r="B5" s="3">
-        <f>'Avoided Def'!B13*1000000</f>
-        <v>75884.477421999734</v>
+        <f>'Avoided Def'!B13*10^9</f>
+        <v>75884477.421999738</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1537,8 +1542,8 @@
         <v>7</v>
       </c>
       <c r="B7" s="3">
-        <f>'Forest Rest'!B12*1000000</f>
-        <v>1144.0518394431674</v>
+        <f>'Forest Rest'!B12*10^9</f>
+        <v>1144051.8394431674</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>

</xml_diff>

<commit_message>
WRI edits to land use files
</commit_message>
<xml_diff>
--- a/InputData/land/CSpULApYbP/CO2 Sequestered per Unit Land Area per Year by Pol.xlsx
+++ b/InputData/land/CSpULApYbP/CO2 Sequestered per Unit Land Area per Year by Pol.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\Brazil\Models\eps-brazil\InputData\land\CSpULApYbP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-brazil\InputData\land\CSpULApYbP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="315" yWindow="315" windowWidth="18825" windowHeight="6555" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -27,12 +27,23 @@
     <definedName name="C_to_CO2">'[1]Conversion Factors'!$A$4</definedName>
     <definedName name="grams_per_ton">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="67">
   <si>
     <t>CSpULApYbP CO2 Sequestered per Unit Land Area per Year by Policy</t>
   </si>
@@ -73,9 +84,6 @@
     <t>Gg de CO2 per acre per year</t>
   </si>
   <si>
-    <t>Gg/ Co2 per yr</t>
-  </si>
-  <si>
     <t>Total area reforested:</t>
   </si>
   <si>
@@ -88,7 +96,142 @@
     <t>Gg Co2 per acre per year</t>
   </si>
   <si>
-    <t>Co2 sequestred:</t>
+    <t>Afforestation and Reforestation</t>
+  </si>
+  <si>
+    <t>Brazilian Ministry of Science, Technology, Innovation and Communication (MCTIC)</t>
+  </si>
+  <si>
+    <t>Report: "Opções de mitigação de gases de efeito estufa em setores-chave do Brasil"</t>
+  </si>
+  <si>
+    <t>Version: "Modelagem Setorial  de opções de baixo carbono para agricultura, florestas e outros usos do solo (AFOLU)"</t>
+  </si>
+  <si>
+    <t>http://www.mctic.gov.br/mctic/export/sites/institucional/ciencia/SEPED/clima/arquivos/projeto_opcoes_mitigacao/publicacoes/AFOLU.pdf</t>
+  </si>
+  <si>
+    <t>Avoided Deforestation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forest Restoration </t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>Forest set asides, Improved forest management and peatland restoration policies</t>
+  </si>
+  <si>
+    <t>are not used in the BR version of the model.</t>
+  </si>
+  <si>
+    <t>Page 173</t>
+  </si>
+  <si>
+    <t>Taking the values from the report, planted forests remove an average of 34,000 Gg of CO2 per year</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>Page 172, figure 57</t>
+  </si>
+  <si>
+    <t>Restored area:</t>
+  </si>
+  <si>
+    <t>The removal for that activity does not occur equally over time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">However, for the purpose of meeting the variable, the accumulated </t>
+  </si>
+  <si>
+    <t xml:space="preserve">removal value was divided by the years of the report </t>
+  </si>
+  <si>
+    <t>project in question, reaching an annual removal value.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It should be noted that deforestation occurs in vegetation formations with </t>
+  </si>
+  <si>
+    <t>different levels of carbon. Stipulating how much is emitted per unit area</t>
+  </si>
+  <si>
+    <t>is an aggregation exercise, due to several existing details.</t>
+  </si>
+  <si>
+    <t>Hence, for the BR version, this variable contains data for Afforestation/Reforestation;</t>
+  </si>
+  <si>
+    <t>Afforestation/Reforestation:</t>
+  </si>
+  <si>
+    <t>Avoid deforestation:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forest restoration  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">implanted area per year </t>
+  </si>
+  <si>
+    <t>Applying this to the area implemented per year, stipulated in the PLANAbPiaSY:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For the purpose of aligning the database used - 'Options Report' with EPS, removals were not </t>
+  </si>
+  <si>
+    <t xml:space="preserve">considered to be cumulative, they occur at the time of implementation of the policy - in this </t>
+  </si>
+  <si>
+    <t>case, at the time of transition from land use to reforestation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since there is no deforestation control policy in conventional policies, </t>
+  </si>
+  <si>
+    <t>the removal value by the policy was disregarded.</t>
+  </si>
+  <si>
+    <t>case, at the time of transition from land use to Forest restoration.</t>
+  </si>
+  <si>
+    <t>and Forest restoration. Avoid deforestation  will be dealt with separately in specific scenarios.</t>
+  </si>
+  <si>
+    <t>CO2 sequestred:</t>
+  </si>
+  <si>
+    <t>Gg/ CO2 per yr</t>
+  </si>
+  <si>
+    <t>Report: "Quarta Comunicação Nacional e Relatórios De Atualização Bienal Do Brasil à Convenção-Quadro das Nações Unidas Sobre Mudança do Clima"</t>
+  </si>
+  <si>
+    <t>Version: "Relatório de referência para consulta pública - LULUCF"</t>
+  </si>
+  <si>
+    <t>http://antigo.mctic.gov.br/mctic/opencms/ciencia/SEPED/clima/Comunicacao_Nacional/Comunicacao_Nacional.html</t>
+  </si>
+  <si>
+    <t>considered, that is, how much was emitted for a considered area.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Therefore, it was stipulated how much is left to be emitted when failing to </t>
+  </si>
+  <si>
+    <t>deforest a fraction in a specific scenario.</t>
+  </si>
+  <si>
+    <t>Annual average</t>
+  </si>
+  <si>
+    <t>Gg de CO2</t>
+  </si>
+  <si>
+    <t>acre</t>
   </si>
   <si>
     <t>Total área</t>
@@ -97,136 +240,10 @@
     <t>Km²</t>
   </si>
   <si>
-    <t>acre</t>
-  </si>
-  <si>
-    <t>Gg de CO2</t>
-  </si>
-  <si>
     <t>Emissions:</t>
   </si>
   <si>
-    <t>Afforestation and Reforestation</t>
-  </si>
-  <si>
-    <t>Brazilian Ministry of Science, Technology, Innovation and Communication (MCTIC)</t>
-  </si>
-  <si>
-    <t>Report: "Opções de mitigação de gases de efeito estufa em setores-chave do Brasil"</t>
-  </si>
-  <si>
-    <t>Version: "Modelagem Setorial  de opções de baixo carbono para agricultura, florestas e outros usos do solo (AFOLU)"</t>
-  </si>
-  <si>
-    <t>http://www.mctic.gov.br/mctic/export/sites/institucional/ciencia/SEPED/clima/arquivos/projeto_opcoes_mitigacao/publicacoes/AFOLU.pdf</t>
-  </si>
-  <si>
-    <t>Avoided Deforestation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forest Restoration </t>
-  </si>
-  <si>
-    <t>Notes:</t>
-  </si>
-  <si>
-    <t>Forest set asides, Improved forest management and peatland restoration policies</t>
-  </si>
-  <si>
-    <t>are not used in the BR version of the model.</t>
-  </si>
-  <si>
-    <t>Page 173</t>
-  </si>
-  <si>
-    <t>Taking the values from the report, planted forests remove an average of 34,000 Gg of CO2 per year</t>
-  </si>
-  <si>
-    <t>=</t>
-  </si>
-  <si>
-    <t>Page 172, figure 57</t>
-  </si>
-  <si>
-    <t>Restored area:</t>
-  </si>
-  <si>
-    <t>The removal for that activity does not occur equally over time.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">However, for the purpose of meeting the variable, the accumulated </t>
-  </si>
-  <si>
-    <t xml:space="preserve">removal value was divided by the years of the report </t>
-  </si>
-  <si>
-    <t>project in question, reaching an annual removal value.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It should be noted that deforestation occurs in vegetation formations with </t>
-  </si>
-  <si>
-    <t>different levels of carbon. Stipulating how much is emitted per unit area</t>
-  </si>
-  <si>
-    <t>is an aggregation exercise, due to several existing details.</t>
-  </si>
-  <si>
-    <t>Annual average</t>
-  </si>
-  <si>
-    <t>Page 172, 216</t>
-  </si>
-  <si>
-    <t>Hence, for the BR version, this variable contains data for Afforestation/Reforestation;</t>
-  </si>
-  <si>
-    <t>Avoid deforestation, Forest restoration.</t>
-  </si>
-  <si>
-    <t>Afforestation/Reforestation:</t>
-  </si>
-  <si>
-    <t>For the Afforestation/Reforestation policy, this variable represents the amount of</t>
-  </si>
-  <si>
-    <t>CO2 sequestered each year by the new forest that is growing on a given acre.</t>
-  </si>
-  <si>
-    <t>Avoid deforestation:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Starting from an average value of how much CO2 would be emitted through deforestation for </t>
-  </si>
-  <si>
-    <t>an area, the value of what is not being emitted by area is obtained.</t>
-  </si>
-  <si>
-    <t>That is, the CO2 that is leaving to go to atmosphere to prevent deforestation by area.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forest restoration  </t>
-  </si>
-  <si>
-    <t>For the Forest restoration  policy, this variable represents the amount of</t>
-  </si>
-  <si>
-    <t>CO2 sequestered each year by the forest that is growing on a given acre.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The average annual emission per area that is deforested in the reference scenario was </t>
-  </si>
-  <si>
-    <t>considered, that is, how much was emitted for a considered area.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Therefore, it was stipulated how much is left to be emitted when failing to </t>
-  </si>
-  <si>
-    <t>deforest a fraction in a specific scenario.</t>
-  </si>
-  <si>
-    <t>It is noted that both scenarios considered in the report have deforestation.</t>
+    <t xml:space="preserve">The average annual emission per area that is deforested in the BAU scenario was </t>
   </si>
 </sst>
 </file>
@@ -372,7 +389,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -389,7 +406,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -427,54 +443,10 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="About"/>
-      <sheetName val="CO2 Aff &amp; Ref"/>
-      <sheetName val="VFC-PIIiCRfAaREY"/>
-      <sheetName val="Lost Value Aff &amp; Ref"/>
-      <sheetName val="VFC-LVpIIiCAbAaR"/>
-      <sheetName val="One Time Cost Aff &amp; Ref"/>
-      <sheetName val="VFC-OTCpIIiCAbAaR"/>
-      <sheetName val="Ongoing Cost Aff &amp; Ref"/>
-      <sheetName val="VFC-OCpMCAbAaR"/>
-      <sheetName val="CO2 Set Asides"/>
-      <sheetName val="VFC-PACRfFSA"/>
-      <sheetName val="Lost Value Set Asides"/>
-      <sheetName val="VFC-LVpMCAbFSA"/>
-      <sheetName val="CO2 Avoided Deforestation"/>
-      <sheetName val="VFC-PACRfAD"/>
-      <sheetName val="Lost Value Avoided Deforestatio"/>
-      <sheetName val="VFC-LVpMCAbAD"/>
-      <sheetName val="County Data"/>
-      <sheetName val="Forest Mgmt Costs"/>
       <sheetName val="Conversion Factors"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19">
-        <row r="4">
-          <cell r="A4">
-            <v>3.6666666666666665</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -767,311 +739,283 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B59"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" customWidth="1"/>
-    <col min="2" max="2" width="66.7109375" customWidth="1"/>
+    <col min="1" max="1" width="10.46484375" customWidth="1"/>
+    <col min="2" max="2" width="66.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="B4" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="14.25" x14ac:dyDescent="0.45">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B4" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" s="5">
         <v>2017</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B8" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B9" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="B9" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" s="6" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10"/>
-      <c r="B10" s="10"/>
-    </row>
-    <row r="11" spans="1:2" s="6" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A11"/>
-    </row>
-    <row r="12" spans="1:2" s="6" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B11" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A12"/>
-      <c r="B12" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" s="6" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A13"/>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" s="6" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
+      <c r="B13" s="5">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A14"/>
-      <c r="B14" s="5">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A15"/>
       <c r="B15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A16"/>
+      <c r="B16" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A17"/>
+      <c r="B17" s="12"/>
+    </row>
+    <row r="18" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A18"/>
+      <c r="B18" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A19"/>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A20"/>
+      <c r="B20" s="5">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A21"/>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A22"/>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A23"/>
+      <c r="B23" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B24" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16"/>
-      <c r="B16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" s="6" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A17"/>
-      <c r="B17" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" s="6" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A18" s="1"/>
-      <c r="B18" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="6"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A31" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="6"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A33" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="6"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A34" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="6"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="6"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A36" s="8" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19"/>
-      <c r="B19"/>
-    </row>
-    <row r="20" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20"/>
-      <c r="B20" s="10"/>
-    </row>
-    <row r="21" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21"/>
-      <c r="B21" s="1"/>
-    </row>
-    <row r="22" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22"/>
-      <c r="B22" s="12"/>
-    </row>
-    <row r="23" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23"/>
-      <c r="B23" s="7"/>
-    </row>
-    <row r="24" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24"/>
-      <c r="B24" s="13"/>
-    </row>
-    <row r="25" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25"/>
-      <c r="B25" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26"/>
-      <c r="B26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27"/>
-      <c r="B27" s="5">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28"/>
-      <c r="B28" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29"/>
-      <c r="B29" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30"/>
-      <c r="B30" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B36" s="6"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A37" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="6"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
         <v>48</v>
       </c>
-      <c r="B37" s="6"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
+      <c r="B38" s="6"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A39" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="6"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
       <c r="B39" s="6"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="15" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A40" s="8"/>
+      <c r="B40" s="6"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A42" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="6"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" s="6"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="6"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
         <v>50</v>
       </c>
-      <c r="B40" s="6"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>51</v>
-      </c>
-      <c r="B41" s="6"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>52</v>
-      </c>
-      <c r="B42" s="6"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B44" s="6"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>54</v>
-      </c>
       <c r="B45" s="6"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="s">
-        <v>55</v>
-      </c>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A46" s="6"/>
       <c r="B46" s="6"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="s">
-        <v>56</v>
-      </c>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A47" s="6"/>
       <c r="B47" s="6"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>57</v>
-      </c>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A49" s="6"/>
       <c r="B49" s="6"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>58</v>
-      </c>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A50" s="6"/>
       <c r="B50" s="6"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
-        <v>59</v>
-      </c>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A51" s="6"/>
       <c r="B51" s="6"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="6"/>
-      <c r="B53" s="6"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="6"/>
-      <c r="B54" s="6"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="6"/>
-      <c r="B55" s="6"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="6"/>
-      <c r="B56" s="6"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="6"/>
-      <c r="B57" s="6"/>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="6"/>
-      <c r="B58" s="6"/>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="6"/>
-      <c r="B59" s="6"/>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B17" r:id="rId1"/>
-    <hyperlink ref="B30" r:id="rId2"/>
-    <hyperlink ref="B8" r:id="rId3"/>
+    <hyperlink ref="B23" r:id="rId1"/>
+    <hyperlink ref="B8" r:id="rId2"/>
+    <hyperlink ref="B16" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1082,62 +1026,76 @@
   <dimension ref="A2:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="14.25" x14ac:dyDescent="0.45">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B15" s="9">
         <v>34000</v>
       </c>
       <c r="C15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" t="s">
         <v>13</v>
       </c>
-      <c r="E15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E16">
         <v>5359980</v>
       </c>
       <c r="F16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="E17">
         <f>E16*G17</f>
         <v>13239150.600000001</v>
       </c>
       <c r="F17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G17">
         <v>2.4700000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="14">
-        <f>B15/E17</f>
-        <v>2.568140587508688E-3</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>17</v>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18">
+        <v>427250.92190322583</v>
+      </c>
+      <c r="F18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" s="6"/>
+      <c r="B19" s="13">
+        <f>B15/E18</f>
+        <v>7.9578529283316907E-2</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1150,115 +1108,114 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A4" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6" s="8"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B10">
+        <v>652321</v>
+      </c>
+      <c r="C10" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="H10" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="B10">
-        <v>376500</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10" t="s">
-        <v>21</v>
       </c>
       <c r="I10">
         <v>2.4700000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="D11" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="E11" s="9">
-        <v>20087</v>
+        <v>24073</v>
       </c>
       <c r="F11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="E12">
-        <v>2008700</v>
+        <f>E11*100</f>
+        <v>2407300</v>
       </c>
       <c r="F12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="14">
+        <v>29</v>
+      </c>
+      <c r="B13" s="13">
         <f>B10/E13</f>
-        <v>7.5884477421999733E-2</v>
-      </c>
-      <c r="C13" s="14" t="s">
+        <v>0.10970696250994989</v>
+      </c>
+      <c r="C13" s="13" t="s">
         <v>12</v>
       </c>
       <c r="E13">
         <f>E12*I10</f>
-        <v>4961489</v>
+        <v>5946031.0000000009</v>
       </c>
       <c r="F13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="14.25" x14ac:dyDescent="0.45">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="8" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1271,53 +1228,53 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="D7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="D8">
         <v>16399999.999999998</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G8">
         <v>2.4700000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="D9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1328,7 +1285,7 @@
         <v>40530000</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B11">
         <f>B10/D10</f>
         <v>4.3473969898840364E-2</v>
@@ -1337,15 +1294,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.25" x14ac:dyDescent="0.45">
-      <c r="A12" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="14">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="13">
         <f>B11/38</f>
         <v>1.1440518394431674E-3</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1361,14 +1318,14 @@
   </sheetPr>
   <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B3:B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="33.46484375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.45">
@@ -1407,7 +1364,7 @@
       </c>
       <c r="B3" s="3">
         <f>'Aff &amp; Ref'!B19*10^9</f>
-        <v>2568140.5875086877</v>
+        <v>79578529.28331691</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1458,7 +1415,7 @@
       </c>
       <c r="B5" s="3">
         <f>'Avoided Def'!B13*10^9</f>
-        <v>75884477.421999738</v>
+        <v>109706962.50994989</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>

</xml_diff>